<commit_message>
New and updated files
</commit_message>
<xml_diff>
--- a/Sales/Kings Shop Property.xlsx
+++ b/Sales/Kings Shop Property.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
   <si>
     <t>Date</t>
   </si>
@@ -148,6 +148,12 @@
   </si>
   <si>
     <t>SV8</t>
+  </si>
+  <si>
+    <t>SV9</t>
+  </si>
+  <si>
+    <t>Total Received</t>
   </si>
 </sst>
 </file>
@@ -808,29 +814,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M10"/>
+  <dimension ref="A2:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.7265625" style="3"/>
-    <col min="7" max="7" width="9.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="8.7265625" style="3"/>
-    <col min="11" max="11" width="10.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.2265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="8.7265625" style="3"/>
+    <col min="8" max="8" width="9.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="8.7265625" style="3"/>
+    <col min="12" max="12" width="10.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.2265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="37.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -847,31 +851,34 @@
         <v>3</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L3" t="s">
-        <v>0</v>
-      </c>
       <c r="M3" t="s">
+        <v>0</v>
+      </c>
+      <c r="N3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -893,8 +900,11 @@
       <c r="G4" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.75">
+      <c r="H4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -902,32 +912,36 @@
         <v>-18</v>
       </c>
       <c r="C5">
-        <f>C4+B5</f>
+        <f t="shared" ref="C5:C11" si="0">C4+B5</f>
         <v>382</v>
       </c>
       <c r="D5" s="3">
-        <f>IF(LEFT(A5,3)="W/O",0,(D$4/400)*B5)</f>
+        <f t="shared" ref="D5:D11" si="1">IF(LEFT(A5,3)="W/O",0,(D$4/400)*B5)</f>
         <v>-17.928000000000001</v>
       </c>
       <c r="E5" s="3">
         <v>60</v>
       </c>
       <c r="F5" s="3">
+        <f>F4+E5</f>
+        <v>60</v>
+      </c>
+      <c r="G5" s="3">
         <f>E5+D5</f>
         <v>42.072000000000003</v>
       </c>
-      <c r="G5" s="3">
-        <f>G4+F5</f>
+      <c r="H5" s="3">
+        <f>H4+G5</f>
         <v>42.072000000000003</v>
       </c>
-      <c r="K5" s="3">
+      <c r="L5" s="3">
         <v>63</v>
       </c>
-      <c r="L5" s="1">
+      <c r="M5" s="1">
         <v>42615</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -935,35 +949,39 @@
         <v>-12</v>
       </c>
       <c r="C6">
-        <f>C5+B6</f>
+        <f t="shared" si="0"/>
         <v>370</v>
       </c>
       <c r="D6" s="3">
-        <f>IF(LEFT(A6,3)="W/O",0,(D$4/400)*B6)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E6" s="3">
         <v>0</v>
       </c>
       <c r="F6" s="3">
-        <f t="shared" ref="F6:F10" si="0">E6+D6</f>
-        <v>0</v>
+        <f t="shared" ref="F6:F11" si="2">F5+E6</f>
+        <v>60</v>
       </c>
       <c r="G6" s="3">
-        <f t="shared" ref="G6:G10" si="1">G5+F6</f>
+        <f t="shared" ref="G6:G11" si="3">E6+D6</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="3">
+        <f t="shared" ref="H6:H11" si="4">H5+G6</f>
         <v>42.072000000000003</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="L6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="L6" s="1">
+      <c r="M6" s="1">
         <v>42615</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -971,32 +989,36 @@
         <v>-23</v>
       </c>
       <c r="C7">
-        <f>C6+B7</f>
+        <f t="shared" si="0"/>
         <v>347</v>
       </c>
       <c r="D7" s="3">
-        <f>IF(LEFT(A7,3)="W/O",0,(D$4/400)*B7)</f>
+        <f t="shared" si="1"/>
         <v>-22.908000000000001</v>
       </c>
       <c r="E7" s="3">
         <v>80.5</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
+        <v>140.5</v>
+      </c>
+      <c r="G7" s="3">
+        <f t="shared" si="3"/>
         <v>57.591999999999999</v>
       </c>
-      <c r="G7" s="3">
-        <f t="shared" si="1"/>
+      <c r="H7" s="3">
+        <f t="shared" si="4"/>
         <v>99.664000000000001</v>
       </c>
-      <c r="K7" s="3">
+      <c r="L7" s="3">
         <v>80.5</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -1004,35 +1026,39 @@
         <v>-6</v>
       </c>
       <c r="C8">
-        <f>C7+B8</f>
+        <f t="shared" si="0"/>
         <v>341</v>
       </c>
       <c r="D8" s="3">
-        <f>IF(LEFT(A8,3)="W/O",0,(D$4/400)*B8)</f>
+        <f t="shared" si="1"/>
         <v>-5.976</v>
       </c>
       <c r="E8" s="3">
         <v>21</v>
       </c>
       <c r="F8" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
+        <v>161.5</v>
+      </c>
+      <c r="G8" s="3">
+        <f t="shared" si="3"/>
         <v>15.024000000000001</v>
       </c>
-      <c r="G8" s="3">
-        <f t="shared" si="1"/>
+      <c r="H8" s="3">
+        <f t="shared" si="4"/>
         <v>114.688</v>
       </c>
-      <c r="J8" s="3">
+      <c r="K8" s="3">
         <v>1.5</v>
       </c>
-      <c r="K8" s="3">
+      <c r="L8" s="3">
         <v>22.5</v>
       </c>
-      <c r="L8" s="1">
+      <c r="M8" s="1">
         <v>42620</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -1040,35 +1066,39 @@
         <v>-4</v>
       </c>
       <c r="C9">
-        <f>C8+B9</f>
+        <f t="shared" si="0"/>
         <v>337</v>
       </c>
       <c r="D9" s="3">
-        <f>IF(LEFT(A9,3)="W/O",0,(D$4/400)*B9)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E9" s="3">
         <v>0</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>161.5</v>
       </c>
       <c r="G9" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="3">
+        <f t="shared" si="4"/>
         <v>114.688</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="L9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="L9" s="1">
+      <c r="M9" s="1">
         <v>42629</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -1076,33 +1106,74 @@
         <v>-4</v>
       </c>
       <c r="C10">
-        <f>C9+B10</f>
+        <f t="shared" si="0"/>
         <v>333</v>
       </c>
       <c r="D10" s="3">
-        <f>IF(LEFT(A10,3)="W/O",0,(D$4/400)*B10)</f>
+        <f t="shared" si="1"/>
         <v>-3.984</v>
       </c>
       <c r="E10" s="3">
         <v>16</v>
       </c>
       <c r="F10" s="3">
+        <f t="shared" si="2"/>
+        <v>177.5</v>
+      </c>
+      <c r="G10" s="3">
+        <f t="shared" si="3"/>
+        <v>12.016</v>
+      </c>
+      <c r="H10" s="3">
+        <f t="shared" si="4"/>
+        <v>126.70400000000001</v>
+      </c>
+      <c r="L10" s="3">
+        <v>16</v>
+      </c>
+      <c r="M10" s="1">
+        <v>42677</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11">
+        <v>-9</v>
+      </c>
+      <c r="C11">
         <f t="shared" si="0"/>
-        <v>12.016</v>
-      </c>
-      <c r="G10" s="3">
+        <v>324</v>
+      </c>
+      <c r="D11" s="3">
         <f t="shared" si="1"/>
-        <v>126.70400000000001</v>
-      </c>
-      <c r="K10" s="3">
-        <v>16</v>
-      </c>
-      <c r="L10" s="1">
-        <v>42677</v>
+        <v>-8.9640000000000004</v>
+      </c>
+      <c r="E11" s="3">
+        <v>31.5</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" si="2"/>
+        <v>209</v>
+      </c>
+      <c r="G11" s="3">
+        <f t="shared" si="3"/>
+        <v>22.536000000000001</v>
+      </c>
+      <c r="H11" s="3">
+        <f t="shared" si="4"/>
+        <v>149.24</v>
+      </c>
+      <c r="L11" s="3">
+        <v>31.5</v>
+      </c>
+      <c r="M11" s="1">
+        <v>42678</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="gb+xFsYfOwR8bIostzpgrv6Q2agDFUMhKx+6SIz5mHMgKoIctcGMP5Qpr5XtVLQpLyg5KO/l7+5PjVL4h1cQ9g==" saltValue="dTPtStuzCGqqHRS04yPC6Q==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>